<commit_message>
Adding possibilitie to put tape generated from turing machine
</commit_message>
<xml_diff>
--- a/biomorph_characteristics.xlsx
+++ b/biomorph_characteristics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,22 +505,22 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1.261780978028505</v>
+        <v>1.196158711389379</v>
       </c>
       <c r="E2" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F2" t="n">
-        <v>0.03222222222222222</v>
+        <v>0.02222222222222222</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1765897806139527</v>
+        <v>0.1474055462380178</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9711111111111111</v>
+        <v>0.9733333333333334</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9488888888888889</v>
+        <v>0.9733333333333334</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -547,19 +547,19 @@
         <v>1.229715809318648</v>
       </c>
       <c r="E3" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" t="n">
-        <v>0.02444444444444445</v>
+        <v>0.02333333333333333</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1544244591385928</v>
+        <v>0.1509598916563234</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9688888888888889</v>
+        <v>0.9711111111111111</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9644444444444444</v>
+        <v>0.9711111111111111</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -583,22 +583,22 @@
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>1.261780978028505</v>
+        <v>1.229715809318648</v>
       </c>
       <c r="E4" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F4" t="n">
-        <v>0.02</v>
+        <v>0.02555555555555556</v>
       </c>
       <c r="G4" t="n">
-        <v>0.14</v>
+        <v>0.1578051619428289</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9777777777777777</v>
+        <v>0.9755555555555555</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9688888888888889</v>
+        <v>0.9577777777777777</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -622,22 +622,22 @@
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>1.261780978028505</v>
+        <v>1.229715809318648</v>
       </c>
       <c r="E5" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02555555555555556</v>
+        <v>0.02888888888888889</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1578051619428289</v>
+        <v>0.1674942416552113</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9755555555555555</v>
+        <v>0.9777777777777777</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9711111111111111</v>
+        <v>0.9644444444444444</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -661,22 +661,22 @@
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.292481250360576</v>
+        <v>1.229715809318648</v>
       </c>
       <c r="E6" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02444444444444445</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1544244591385928</v>
+        <v>0.1611072796479276</v>
       </c>
       <c r="H6" t="n">
-        <v>0.96</v>
+        <v>0.9644444444444444</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9733333333333334</v>
+        <v>0.9644444444444444</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -703,19 +703,19 @@
         <v>1.261780978028505</v>
       </c>
       <c r="E7" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02333333333333333</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1509598916563234</v>
+        <v>0.1795054935711501</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9622222222222222</v>
+        <v>0.9688888888888889</v>
       </c>
       <c r="I7" t="n">
-        <v>0.9711111111111111</v>
+        <v>0.96</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -739,22 +739,22 @@
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>1.261780978028505</v>
+        <v>1.292481250360576</v>
       </c>
       <c r="E8" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01777777777777778</v>
+        <v>0.02333333333333333</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1321428333094978</v>
+        <v>0.1509598916563234</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9733333333333334</v>
+        <v>0.9622222222222222</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9733333333333334</v>
+        <v>0.9622222222222222</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -778,22 +778,22 @@
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>1.196158711389378</v>
+        <v>1.292481250360576</v>
       </c>
       <c r="E9" t="n">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F9" t="n">
-        <v>0.01777777777777778</v>
+        <v>0.03222222222222222</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1321428333094978</v>
+        <v>0.1765897806139527</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9644444444444444</v>
+        <v>0.9577777777777777</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9777777777777777</v>
+        <v>0.9711111111111111</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -817,22 +817,22 @@
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>1.196158711389378</v>
+        <v>1.292481250360576</v>
       </c>
       <c r="E10" t="n">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01555555555555556</v>
+        <v>0.03444444444444444</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1237480514873409</v>
+        <v>0.1823678280052653</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9688888888888889</v>
+        <v>0.9488888888888889</v>
       </c>
       <c r="I10" t="n">
-        <v>0.9733333333333334</v>
+        <v>0.9622222222222222</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -856,22 +856,22 @@
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>1.196158711389378</v>
+        <v>1.292481250360576</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F11" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.03888888888888889</v>
       </c>
       <c r="G11" t="n">
-        <v>0.114697670227235</v>
+        <v>0.1933301404589479</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9733333333333334</v>
+        <v>0.9311111111111111</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9777777777777777</v>
+        <v>0.9533333333333334</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -895,22 +895,22 @@
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>1.196158711389378</v>
+        <v>1.229715809318646</v>
       </c>
       <c r="E12" t="n">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.03777777777777778</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1146976702272351</v>
+        <v>0.1906583784782369</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9733333333333334</v>
+        <v>0.9511111111111111</v>
       </c>
       <c r="I12" t="n">
-        <v>0.9822222222222222</v>
+        <v>0.9422222222222222</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -934,29 +934,2681 @@
         <v>12</v>
       </c>
       <c r="D13" t="n">
+        <v>1.229715809318646</v>
+      </c>
+      <c r="E13" t="n">
+        <v>31</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.03444444444444444</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.1823678280052652</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.9488888888888889</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>13</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.229715809318646</v>
+      </c>
+      <c r="E14" t="n">
+        <v>28</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.03111111111111111</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.1736179998633299</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.9377777777777778</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>14</v>
+      </c>
+      <c r="D15" t="n">
         <v>1.196158711389378</v>
       </c>
-      <c r="E13" t="n">
-        <v>12</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.01333333333333333</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.1146976702272351</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.9733333333333334</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.9822222222222222</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>30</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.1795054935711501</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.9422222222222222</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>15</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.196158711389378</v>
+      </c>
+      <c r="E16" t="n">
+        <v>34</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.03777777777777778</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.1906583784782369</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.9511111111111111</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>16</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.261780978028505</v>
+      </c>
+      <c r="E17" t="n">
+        <v>30</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.1795054935711501</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.9422222222222222</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>17</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.261780978028505</v>
+      </c>
+      <c r="E18" t="n">
+        <v>40</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.04444444444444445</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.2060804110110156</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.9288888888888889</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.9466666666666667</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>18</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.261780978028505</v>
+      </c>
+      <c r="E19" t="n">
+        <v>28</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.03111111111111111</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.1736179998633299</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>19</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.350219859070544</v>
+      </c>
+      <c r="E20" t="n">
+        <v>30</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.1795054935711501</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.9511111111111111</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>20</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.377443751081733</v>
+      </c>
+      <c r="E21" t="n">
+        <v>36</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.1959591794226543</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.9466666666666667</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.9466666666666667</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>21</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.4036774610288</v>
+      </c>
+      <c r="E22" t="n">
+        <v>42</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.04666666666666667</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.210923893594085</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>22</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.4036774610288</v>
+      </c>
+      <c r="E23" t="n">
+        <v>58</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.06444444444444444</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.245542986103638</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.9244444444444444</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.9244444444444444</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>23</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.453445297804257</v>
+      </c>
+      <c r="E24" t="n">
+        <v>44</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.04888888888888889</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.2156357239237014</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.9288888888888889</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.9377777777777778</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>24</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.377443751081733</v>
+      </c>
+      <c r="E25" t="n">
+        <v>52</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.05777777777777778</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.2333227510827856</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.9288888888888889</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.9422222222222222</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>25</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.377443751081733</v>
+      </c>
+      <c r="E26" t="n">
+        <v>58</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.06444444444444444</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.245542986103638</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.8977777777777778</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.9244444444444444</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>26</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1.4036774610288</v>
+      </c>
+      <c r="E27" t="n">
+        <v>62</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.06888888888888889</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.2532650980228883</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.9066666666666666</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.8977777777777778</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>27</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.428990497563784</v>
+      </c>
+      <c r="E28" t="n">
+        <v>88</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.09777777777777778</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.2970139457173978</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.8755555555555555</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.8977777777777778</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>28</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.522197059679226</v>
+      </c>
+      <c r="E29" t="n">
+        <v>64</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.07111111111111111</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.2570103519075727</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.8933333333333333</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>29</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.604726682814473</v>
+      </c>
+      <c r="E30" t="n">
+        <v>102</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.1133333333333333</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.3169998247458332</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.8533333333333334</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.8977777777777778</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>30</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.623963756721791</v>
+      </c>
+      <c r="E31" t="n">
+        <v>74</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.08222222222222222</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.2747029821371834</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.8533333333333334</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.8711111111111111</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>31</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1.584962500721153</v>
+      </c>
+      <c r="E32" t="n">
+        <v>80</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.08888888888888889</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.2845832994414599</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.8577777777777778</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.8844444444444445</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>32</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1.564641508472482</v>
+      </c>
+      <c r="E33" t="n">
+        <v>68</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.07555555555555556</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.2642856666189957</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.8844444444444445</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.8933333333333333</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>33</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1.522197059679224</v>
+      </c>
+      <c r="E34" t="n">
+        <v>70</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.07777777777777778</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.2678215731820878</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.9066666666666666</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>34</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1.543731420625169</v>
+      </c>
+      <c r="E35" t="n">
+        <v>68</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.07555555555555556</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.2642856666189957</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.8755555555555555</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.8933333333333333</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>35</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1.564641508472481</v>
+      </c>
+      <c r="E36" t="n">
+        <v>78</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.08666666666666667</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.2813459712801226</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.8711111111111111</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.8844444444444445</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>36</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1.543731420625169</v>
+      </c>
+      <c r="E37" t="n">
+        <v>78</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.08666666666666667</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.2813459712801226</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.8444444444444444</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>37</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1.604726682814473</v>
+      </c>
+      <c r="E38" t="n">
+        <v>84</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.09333333333333334</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.290898989723619</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.8311111111111111</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.8755555555555555</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>38</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1.623963756721791</v>
+      </c>
+      <c r="E39" t="n">
+        <v>104</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.1155555555555556</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.3196912090374123</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.8222222222222222</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>39</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1.623963756721791</v>
+      </c>
+      <c r="E40" t="n">
+        <v>86</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.09555555555555556</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.2939807669865916</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.8711111111111111</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>40</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1.623963756721791</v>
+      </c>
+      <c r="E41" t="n">
+        <v>118</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.1311111111111111</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.3375218328557739</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.8533333333333334</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.8711111111111111</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>41</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1.660964047443679</v>
+      </c>
+      <c r="E42" t="n">
+        <v>86</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.09555555555555556</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.2939807669865916</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.8355555555555556</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.8444444444444444</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>42</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1.564641508472481</v>
+      </c>
+      <c r="E43" t="n">
+        <v>94</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.1044444444444445</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.305836234722336</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.8533333333333334</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>43</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1.584962500721154</v>
+      </c>
+      <c r="E44" t="n">
+        <v>76</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.08444444444444445</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.2780531967931921</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.8755555555555555</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>44</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1.604726682814473</v>
+      </c>
+      <c r="E45" t="n">
+        <v>86</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.09555555555555556</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.2939807669865916</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.8711111111111111</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>45</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1.604726682814473</v>
+      </c>
+      <c r="E46" t="n">
+        <v>80</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.08888888888888889</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.2845832994414599</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>46</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1.660964047443679</v>
+      </c>
+      <c r="E47" t="n">
+        <v>78</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.08666666666666667</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.2813459712801226</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.8533333333333334</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.8844444444444445</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>47</v>
+      </c>
+      <c r="D48" t="n">
+        <v>1.642701109431122</v>
+      </c>
+      <c r="E48" t="n">
+        <v>80</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.08888888888888889</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.2845832994414599</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.8844444444444445</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>48</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1.642701109431122</v>
+      </c>
+      <c r="E49" t="n">
+        <v>88</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.09777777777777778</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.2970139457173978</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>49</v>
+      </c>
+      <c r="D50" t="n">
+        <v>1.678776002309039</v>
+      </c>
+      <c r="E50" t="n">
+        <v>90</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.8444444444444444</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.8533333333333334</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>50</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1.67877600230904</v>
+      </c>
+      <c r="E51" t="n">
+        <v>102</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.1133333333333333</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.3169998247458331</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.8088888888888889</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.8533333333333334</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>51</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1.660964047443679</v>
+      </c>
+      <c r="E52" t="n">
+        <v>96</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.1066666666666667</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.308688984074406</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.8133333333333334</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.8577777777777778</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>52</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1.696158711389378</v>
+      </c>
+      <c r="E53" t="n">
+        <v>98</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.1088888888888889</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.3114997572477899</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.8177777777777778</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.8577777777777778</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>53</v>
+      </c>
+      <c r="D54" t="n">
+        <v>1.729715809318646</v>
+      </c>
+      <c r="E54" t="n">
+        <v>108</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.3249615361854384</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.8133333333333334</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>54</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1.729715809318646</v>
+      </c>
+      <c r="E55" t="n">
+        <v>94</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.1044444444444445</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.305836234722336</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.8355555555555556</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.8488888888888889</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>55</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1.729715809318646</v>
+      </c>
+      <c r="E56" t="n">
+        <v>110</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.1222222222222222</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.3275422882885261</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.8088888888888889</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>56</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1.729715809318646</v>
+      </c>
+      <c r="E57" t="n">
+        <v>86</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.09555555555555556</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.2939807669865916</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.8444444444444444</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.8622222222222222</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>57</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1.713132377351047</v>
+      </c>
+      <c r="E58" t="n">
+        <v>98</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.1088888888888889</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.3114997572477899</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.8177777777777778</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>58</v>
+      </c>
+      <c r="D59" t="n">
+        <v>1.713132377351047</v>
+      </c>
+      <c r="E59" t="n">
+        <v>80</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.08888888888888889</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.2845832994414599</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.8488888888888889</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>59</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1.67877600230904</v>
+      </c>
+      <c r="E60" t="n">
+        <v>74</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.08222222222222222</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.2747029821371834</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.8844444444444445</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>60</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1.67877600230904</v>
+      </c>
+      <c r="E61" t="n">
+        <v>72</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.2712931993250107</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.8844444444444445</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>61</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1.67877600230904</v>
+      </c>
+      <c r="E62" t="n">
+        <v>84</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.09333333333333334</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.290898989723619</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.8577777777777778</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.8844444444444445</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>62</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1.696158711389378</v>
+      </c>
+      <c r="E63" t="n">
+        <v>72</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.2712931993250107</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.8844444444444445</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>63</v>
+      </c>
+      <c r="D64" t="n">
+        <v>1.696158711389378</v>
+      </c>
+      <c r="E64" t="n">
+        <v>80</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.08888888888888889</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.2845832994414599</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0.8488888888888889</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.8844444444444445</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>64</v>
+      </c>
+      <c r="D65" t="n">
+        <v>1.713132377351047</v>
+      </c>
+      <c r="E65" t="n">
+        <v>74</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.08222222222222222</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.2747029821371834</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0.8444444444444444</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.8844444444444445</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>65</v>
+      </c>
+      <c r="D66" t="n">
+        <v>1.642701109431122</v>
+      </c>
+      <c r="E66" t="n">
+        <v>68</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.07555555555555556</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.2642856666189957</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.8933333333333333</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>66</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1.604726682814473</v>
+      </c>
+      <c r="E67" t="n">
+        <v>58</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.06444444444444444</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.245542986103638</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0.9022222222222223</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>67</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1.584962500721153</v>
+      </c>
+      <c r="E68" t="n">
+        <v>66</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.07333333333333333</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0.2606828639468953</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0.8711111111111111</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0.9066666666666666</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>68</v>
+      </c>
+      <c r="D69" t="n">
+        <v>1.604726682814473</v>
+      </c>
+      <c r="E69" t="n">
+        <v>58</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.06444444444444444</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0.245542986103638</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0.9066666666666666</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>69</v>
+      </c>
+      <c r="D70" t="n">
+        <v>1.62396375672179</v>
+      </c>
+      <c r="E70" t="n">
+        <v>64</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.07111111111111111</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.2570103519075726</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0.8844444444444445</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0.9066666666666666</v>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>70</v>
+      </c>
+      <c r="D71" t="n">
+        <v>1.604726682814473</v>
+      </c>
+      <c r="E71" t="n">
+        <v>62</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.06888888888888889</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0.2532650980228883</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0.8711111111111111</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0.9111111111111111</v>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>71</v>
+      </c>
+      <c r="D72" t="n">
+        <v>1.604726682814473</v>
+      </c>
+      <c r="E72" t="n">
+        <v>70</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.07777777777777778</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0.2678215731820878</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0.8533333333333334</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0.8977777777777778</v>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>72</v>
+      </c>
+      <c r="D73" t="n">
+        <v>1.604726682814473</v>
+      </c>
+      <c r="E73" t="n">
+        <v>68</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.07555555555555556</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0.2642856666189957</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0.8977777777777778</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>73</v>
+      </c>
+      <c r="D74" t="n">
+        <v>1.604726682814473</v>
+      </c>
+      <c r="E74" t="n">
+        <v>50</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0.2290614236454256</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0.9066666666666666</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0.9155555555555556</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>74</v>
+      </c>
+      <c r="D75" t="n">
+        <v>1.543731420625168</v>
+      </c>
+      <c r="E75" t="n">
+        <v>46</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.05111111111111111</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0.2202243524955829</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>75</v>
+      </c>
+      <c r="D76" t="n">
+        <v>1.499999999999998</v>
+      </c>
+      <c r="E76" t="n">
+        <v>40</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.04444444444444445</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.2060804110110157</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0.9377777777777778</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>76</v>
+      </c>
+      <c r="D77" t="n">
+        <v>1.499999999999998</v>
+      </c>
+      <c r="E77" t="n">
+        <v>42</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.04666666666666667</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.210923893594085</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.9333333333333333</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0.9422222222222222</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>77</v>
+      </c>
+      <c r="D78" t="n">
+        <v>1.453445297804257</v>
+      </c>
+      <c r="E78" t="n">
+        <v>30</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0.1795054935711501</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0.9422222222222222</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0.9422222222222222</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>78</v>
+      </c>
+      <c r="D79" t="n">
+        <v>1.350219859070545</v>
+      </c>
+      <c r="E79" t="n">
+        <v>24</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.02666666666666667</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0.1611072796479276</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0.9466666666666667</v>
+      </c>
+      <c r="I79" t="n">
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>79</v>
+      </c>
+      <c r="D80" t="n">
+        <v>1.499999999999998</v>
+      </c>
+      <c r="E80" t="n">
+        <v>20</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.02222222222222222</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0.1474055462380178</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0.9644444444444444</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Semente1-Regra1-B3/S23</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>B3/S23</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>80</v>
+      </c>
+      <c r="D81" t="n">
+        <v>1.499999999999998</v>
+      </c>
+      <c r="E81" t="n">
+        <v>20</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.02222222222222222</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0.1474055462380178</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0.9644444444444444</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Changes in image seed name
</commit_message>
<xml_diff>
--- a/biomorph_characteristics.xlsx
+++ b/biomorph_characteristics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,7 +493,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -505,22 +505,22 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1.196158711389379</v>
+        <v>1.084962500721154</v>
       </c>
       <c r="E2" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
-        <v>0.02222222222222222</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1474055462380178</v>
+        <v>0.1146976702272351</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9733333333333334</v>
+        <v>0.9822222222222222</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9733333333333334</v>
+        <v>0.9822222222222222</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -544,22 +544,22 @@
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>1.229715809318648</v>
+        <v>1.123963756721792</v>
       </c>
       <c r="E3" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
-        <v>0.02333333333333333</v>
+        <v>0.01222222222222222</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1509598916563234</v>
+        <v>0.1098764738521074</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9711111111111111</v>
+        <v>0.9755555555555555</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9711111111111111</v>
+        <v>0.9844444444444445</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -571,7 +571,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -583,22 +583,22 @@
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>1.229715809318648</v>
+        <v>1.123963756721792</v>
       </c>
       <c r="E4" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F4" t="n">
-        <v>0.02555555555555556</v>
+        <v>0.01666666666666667</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1578051619428289</v>
+        <v>0.1280190957978102</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9755555555555555</v>
+        <v>0.9666666666666667</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9577777777777777</v>
+        <v>0.98</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -610,7 +610,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -622,22 +622,22 @@
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>1.229715809318648</v>
+        <v>1.123963756721792</v>
       </c>
       <c r="E5" t="n">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02888888888888889</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1674942416552113</v>
+        <v>0.114697670227235</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9777777777777777</v>
+        <v>0.9733333333333334</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9644444444444444</v>
+        <v>0.9866666666666667</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -649,7 +649,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -661,22 +661,22 @@
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>1.229715809318648</v>
+        <v>1.123963756721792</v>
       </c>
       <c r="E6" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02666666666666667</v>
+        <v>0.01666666666666667</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1611072796479276</v>
+        <v>0.1280190957978102</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9644444444444444</v>
+        <v>0.9755555555555555</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9644444444444444</v>
+        <v>0.98</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -688,7 +688,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -700,22 +700,22 @@
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>1.261780978028505</v>
+        <v>1.123963756721792</v>
       </c>
       <c r="E7" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F7" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.01777777777777778</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1795054935711501</v>
+        <v>0.1321428333094978</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9688888888888889</v>
+        <v>0.9777777777777777</v>
       </c>
       <c r="I7" t="n">
-        <v>0.96</v>
+        <v>0.9733333333333334</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -727,7 +727,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -739,22 +739,22 @@
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>1.292481250360576</v>
+        <v>1.123963756721792</v>
       </c>
       <c r="E8" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F8" t="n">
-        <v>0.02333333333333333</v>
+        <v>0.02111111111111111</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1509598916563234</v>
+        <v>0.1437547637428598</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9622222222222222</v>
+        <v>0.9755555555555555</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9622222222222222</v>
+        <v>0.9711111111111111</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -766,7 +766,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -778,22 +778,22 @@
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>1.292481250360576</v>
+        <v>1.123963756721792</v>
       </c>
       <c r="E9" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F9" t="n">
-        <v>0.03222222222222222</v>
+        <v>0.01888888888888889</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1765897806139527</v>
+        <v>0.1361326513568001</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9577777777777777</v>
+        <v>0.9622222222222222</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9711111111111111</v>
+        <v>0.98</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -805,7 +805,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -817,22 +817,22 @@
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>1.292481250360576</v>
+        <v>1.229715809318648</v>
       </c>
       <c r="E10" t="n">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F10" t="n">
-        <v>0.03444444444444444</v>
+        <v>0.02222222222222222</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1823678280052653</v>
+        <v>0.1474055462380178</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9488888888888889</v>
+        <v>0.9733333333333334</v>
       </c>
       <c r="I10" t="n">
-        <v>0.9622222222222222</v>
+        <v>0.9688888888888889</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -844,7 +844,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -856,22 +856,22 @@
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>1.292481250360576</v>
+        <v>1.261780978028505</v>
       </c>
       <c r="E11" t="n">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F11" t="n">
-        <v>0.03888888888888889</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1933301404589479</v>
+        <v>0.1611072796479276</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9311111111111111</v>
+        <v>0.9555555555555556</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9533333333333334</v>
+        <v>0.9644444444444444</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -883,7 +883,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -895,22 +895,22 @@
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>1.229715809318646</v>
+        <v>1.261780978028505</v>
       </c>
       <c r="E12" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F12" t="n">
-        <v>0.03777777777777778</v>
+        <v>0.02888888888888889</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1906583784782369</v>
+        <v>0.1674942416552113</v>
       </c>
       <c r="H12" t="n">
         <v>0.9511111111111111</v>
       </c>
       <c r="I12" t="n">
-        <v>0.9422222222222222</v>
+        <v>0.96</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -934,7 +934,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>1.229715809318646</v>
+        <v>1.261780978028505</v>
       </c>
       <c r="E13" t="n">
         <v>31</v>
@@ -943,13 +943,13 @@
         <v>0.03444444444444444</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1823678280052652</v>
+        <v>0.1823678280052653</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.9488888888888889</v>
       </c>
       <c r="I13" t="n">
-        <v>0.9488888888888889</v>
+        <v>0.9533333333333334</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -961,7 +961,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -973,22 +973,22 @@
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>1.229715809318646</v>
+        <v>1.261780978028505</v>
       </c>
       <c r="E14" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F14" t="n">
-        <v>0.03111111111111111</v>
+        <v>0.03444444444444444</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1736179998633299</v>
+        <v>0.1823678280052653</v>
       </c>
       <c r="H14" t="n">
-        <v>0.9377777777777778</v>
+        <v>0.9577777777777777</v>
       </c>
       <c r="I14" t="n">
-        <v>0.9555555555555556</v>
+        <v>0.9488888888888889</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1000,7 +1000,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1012,22 +1012,22 @@
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>1.196158711389378</v>
+        <v>1.261780978028505</v>
       </c>
       <c r="E15" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F15" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.03666666666666667</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1795054935711501</v>
+        <v>0.1879420714534727</v>
       </c>
       <c r="H15" t="n">
-        <v>0.9422222222222222</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="I15" t="n">
-        <v>0.9555555555555556</v>
+        <v>0.9488888888888889</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1039,7 +1039,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1051,22 +1051,22 @@
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>1.196158711389378</v>
+        <v>1.32192809488736</v>
       </c>
       <c r="E16" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F16" t="n">
-        <v>0.03777777777777778</v>
+        <v>0.04333333333333333</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1906583784782369</v>
+        <v>0.2036063740543393</v>
       </c>
       <c r="H16" t="n">
-        <v>0.9511111111111111</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="I16" t="n">
-        <v>0.9555555555555556</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1078,7 +1078,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1090,22 +1090,22 @@
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>1.261780978028505</v>
+        <v>1.350219859070545</v>
       </c>
       <c r="E17" t="n">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="F17" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.05333333333333334</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1795054935711501</v>
+        <v>0.2246973272847029</v>
       </c>
       <c r="H17" t="n">
-        <v>0.9422222222222222</v>
+        <v>0.92</v>
       </c>
       <c r="I17" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.9511111111111111</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1117,7 +1117,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1129,22 +1129,22 @@
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>1.261780978028505</v>
+        <v>1.350219859070545</v>
       </c>
       <c r="E18" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F18" t="n">
-        <v>0.04444444444444445</v>
+        <v>0.04111111111111111</v>
       </c>
       <c r="G18" t="n">
-        <v>0.2060804110110156</v>
+        <v>0.1985471925118081</v>
       </c>
       <c r="H18" t="n">
-        <v>0.9288888888888889</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="I18" t="n">
-        <v>0.9466666666666667</v>
+        <v>0.9488888888888889</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1156,7 +1156,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1168,19 +1168,19 @@
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>1.261780978028505</v>
+        <v>1.32192809488736</v>
       </c>
       <c r="E19" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F19" t="n">
-        <v>0.03111111111111111</v>
+        <v>0.03777777777777778</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1736179998633299</v>
+        <v>0.1906583784782369</v>
       </c>
       <c r="H19" t="n">
-        <v>0.9555555555555556</v>
+        <v>0.9422222222222222</v>
       </c>
       <c r="I19" t="n">
         <v>0.96</v>
@@ -1195,7 +1195,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1207,7 +1207,7 @@
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>1.350219859070544</v>
+        <v>1.292481250360576</v>
       </c>
       <c r="E20" t="n">
         <v>30</v>
@@ -1219,10 +1219,10 @@
         <v>0.1795054935711501</v>
       </c>
       <c r="H20" t="n">
-        <v>0.9511111111111111</v>
+        <v>0.9422222222222222</v>
       </c>
       <c r="I20" t="n">
-        <v>0.96</v>
+        <v>0.9555555555555556</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1234,7 +1234,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1246,22 +1246,22 @@
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>1.377443751081733</v>
+        <v>1.261780978028505</v>
       </c>
       <c r="E21" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F21" t="n">
-        <v>0.04</v>
+        <v>0.03555555555555556</v>
       </c>
       <c r="G21" t="n">
-        <v>0.1959591794226543</v>
+        <v>0.1851792591644414</v>
       </c>
       <c r="H21" t="n">
         <v>0.9466666666666667</v>
       </c>
       <c r="I21" t="n">
-        <v>0.9466666666666667</v>
+        <v>0.96</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1273,7 +1273,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1285,22 +1285,22 @@
         <v>21</v>
       </c>
       <c r="D22" t="n">
-        <v>1.4036774610288</v>
+        <v>1.292481250360576</v>
       </c>
       <c r="E22" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F22" t="n">
-        <v>0.04666666666666667</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="G22" t="n">
-        <v>0.210923893594085</v>
+        <v>0.1795054935711501</v>
       </c>
       <c r="H22" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.9422222222222222</v>
       </c>
       <c r="I22" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.9422222222222222</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1312,7 +1312,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1324,22 +1324,22 @@
         <v>22</v>
       </c>
       <c r="D23" t="n">
-        <v>1.4036774610288</v>
+        <v>1.292481250360576</v>
       </c>
       <c r="E23" t="n">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="F23" t="n">
-        <v>0.06444444444444444</v>
+        <v>0.04</v>
       </c>
       <c r="G23" t="n">
-        <v>0.245542986103638</v>
+        <v>0.1959591794226543</v>
       </c>
       <c r="H23" t="n">
-        <v>0.9244444444444444</v>
+        <v>0.9555555555555556</v>
       </c>
       <c r="I23" t="n">
-        <v>0.9244444444444444</v>
+        <v>0.9511111111111111</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1351,7 +1351,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1363,22 +1363,22 @@
         <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>1.453445297804257</v>
+        <v>1.292481250360576</v>
       </c>
       <c r="E24" t="n">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="F24" t="n">
-        <v>0.04888888888888889</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="G24" t="n">
-        <v>0.2156357239237014</v>
+        <v>0.1795054935711501</v>
       </c>
       <c r="H24" t="n">
-        <v>0.9288888888888889</v>
+        <v>0.9422222222222222</v>
       </c>
       <c r="I24" t="n">
-        <v>0.9377777777777778</v>
+        <v>0.9511111111111111</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1390,7 +1390,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1402,22 +1402,22 @@
         <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>1.377443751081733</v>
+        <v>1.261780978028505</v>
       </c>
       <c r="E25" t="n">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="F25" t="n">
-        <v>0.05777777777777778</v>
+        <v>0.03555555555555556</v>
       </c>
       <c r="G25" t="n">
-        <v>0.2333227510827856</v>
+        <v>0.1851792591644414</v>
       </c>
       <c r="H25" t="n">
-        <v>0.9288888888888889</v>
+        <v>0.9466666666666667</v>
       </c>
       <c r="I25" t="n">
-        <v>0.9422222222222222</v>
+        <v>0.9511111111111111</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1429,7 +1429,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1441,22 +1441,22 @@
         <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>1.377443751081733</v>
+        <v>1.292481250360576</v>
       </c>
       <c r="E26" t="n">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="F26" t="n">
-        <v>0.06444444444444444</v>
+        <v>0.03555555555555556</v>
       </c>
       <c r="G26" t="n">
-        <v>0.245542986103638</v>
+        <v>0.1851792591644414</v>
       </c>
       <c r="H26" t="n">
-        <v>0.8977777777777778</v>
+        <v>0.9288888888888889</v>
       </c>
       <c r="I26" t="n">
-        <v>0.9244444444444444</v>
+        <v>0.9466666666666667</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1468,7 +1468,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1480,22 +1480,22 @@
         <v>26</v>
       </c>
       <c r="D27" t="n">
-        <v>1.4036774610288</v>
+        <v>1.292481250360576</v>
       </c>
       <c r="E27" t="n">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="F27" t="n">
-        <v>0.06888888888888889</v>
+        <v>0.03555555555555556</v>
       </c>
       <c r="G27" t="n">
-        <v>0.2532650980228883</v>
+        <v>0.1851792591644414</v>
       </c>
       <c r="H27" t="n">
-        <v>0.9066666666666666</v>
+        <v>0.9466666666666667</v>
       </c>
       <c r="I27" t="n">
-        <v>0.8977777777777778</v>
+        <v>0.9511111111111111</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1507,7 +1507,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1519,22 +1519,22 @@
         <v>27</v>
       </c>
       <c r="D28" t="n">
-        <v>1.428990497563784</v>
+        <v>1.292481250360576</v>
       </c>
       <c r="E28" t="n">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="F28" t="n">
-        <v>0.09777777777777778</v>
+        <v>0.02444444444444445</v>
       </c>
       <c r="G28" t="n">
-        <v>0.2970139457173978</v>
+        <v>0.1544244591385928</v>
       </c>
       <c r="H28" t="n">
-        <v>0.8755555555555555</v>
+        <v>0.9511111111111111</v>
       </c>
       <c r="I28" t="n">
-        <v>0.8977777777777778</v>
+        <v>0.96</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1546,7 +1546,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1558,22 +1558,22 @@
         <v>28</v>
       </c>
       <c r="D29" t="n">
-        <v>1.522197059679226</v>
+        <v>1.160964047443679</v>
       </c>
       <c r="E29" t="n">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="F29" t="n">
-        <v>0.07111111111111111</v>
+        <v>0.02</v>
       </c>
       <c r="G29" t="n">
-        <v>0.2570103519075727</v>
+        <v>0.14</v>
       </c>
       <c r="H29" t="n">
-        <v>0.8933333333333333</v>
+        <v>0.96</v>
       </c>
       <c r="I29" t="n">
-        <v>0.88</v>
+        <v>0.9688888888888889</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1585,7 +1585,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1597,22 +1597,22 @@
         <v>29</v>
       </c>
       <c r="D30" t="n">
-        <v>1.604726682814473</v>
+        <v>1.196158711389378</v>
       </c>
       <c r="E30" t="n">
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="F30" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.02444444444444445</v>
       </c>
       <c r="G30" t="n">
-        <v>0.3169998247458332</v>
+        <v>0.1544244591385928</v>
       </c>
       <c r="H30" t="n">
-        <v>0.8533333333333334</v>
+        <v>0.9511111111111111</v>
       </c>
       <c r="I30" t="n">
-        <v>0.8977777777777778</v>
+        <v>0.9688888888888889</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -1624,7 +1624,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1636,22 +1636,22 @@
         <v>30</v>
       </c>
       <c r="D31" t="n">
-        <v>1.623963756721791</v>
+        <v>1.196158711389378</v>
       </c>
       <c r="E31" t="n">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="F31" t="n">
-        <v>0.08222222222222222</v>
+        <v>0.01777777777777778</v>
       </c>
       <c r="G31" t="n">
-        <v>0.2747029821371834</v>
+        <v>0.1321428333094978</v>
       </c>
       <c r="H31" t="n">
-        <v>0.8533333333333334</v>
+        <v>0.9644444444444444</v>
       </c>
       <c r="I31" t="n">
-        <v>0.8711111111111111</v>
+        <v>0.9644444444444444</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -1663,7 +1663,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1675,22 +1675,22 @@
         <v>31</v>
       </c>
       <c r="D32" t="n">
-        <v>1.584962500721153</v>
+        <v>1.160964047443679</v>
       </c>
       <c r="E32" t="n">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="F32" t="n">
-        <v>0.08888888888888889</v>
+        <v>0.01777777777777778</v>
       </c>
       <c r="G32" t="n">
-        <v>0.2845832994414599</v>
+        <v>0.1321428333094978</v>
       </c>
       <c r="H32" t="n">
-        <v>0.8577777777777778</v>
+        <v>0.9644444444444444</v>
       </c>
       <c r="I32" t="n">
-        <v>0.8844444444444445</v>
+        <v>0.9777777777777777</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -1702,7 +1702,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1714,22 +1714,22 @@
         <v>32</v>
       </c>
       <c r="D33" t="n">
-        <v>1.564641508472482</v>
+        <v>1.196158711389378</v>
       </c>
       <c r="E33" t="n">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="F33" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.02</v>
       </c>
       <c r="G33" t="n">
-        <v>0.2642856666189957</v>
+        <v>0.14</v>
       </c>
       <c r="H33" t="n">
-        <v>0.8844444444444445</v>
+        <v>0.96</v>
       </c>
       <c r="I33" t="n">
-        <v>0.8933333333333333</v>
+        <v>0.9777777777777777</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -1741,7 +1741,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1753,22 +1753,22 @@
         <v>33</v>
       </c>
       <c r="D34" t="n">
-        <v>1.522197059679224</v>
+        <v>1.229715809318647</v>
       </c>
       <c r="E34" t="n">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="F34" t="n">
-        <v>0.07777777777777778</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="G34" t="n">
-        <v>0.2678215731820878</v>
+        <v>0.1611072796479276</v>
       </c>
       <c r="H34" t="n">
-        <v>0.88</v>
+        <v>0.9466666666666667</v>
       </c>
       <c r="I34" t="n">
-        <v>0.9066666666666666</v>
+        <v>0.9644444444444444</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -1780,7 +1780,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1792,22 +1792,22 @@
         <v>34</v>
       </c>
       <c r="D35" t="n">
-        <v>1.543731420625169</v>
+        <v>1.229715809318647</v>
       </c>
       <c r="E35" t="n">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="F35" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.03111111111111111</v>
       </c>
       <c r="G35" t="n">
-        <v>0.2642856666189957</v>
+        <v>0.1736179998633299</v>
       </c>
       <c r="H35" t="n">
-        <v>0.8755555555555555</v>
+        <v>0.9377777777777778</v>
       </c>
       <c r="I35" t="n">
-        <v>0.8933333333333333</v>
+        <v>0.9555555555555556</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -1819,7 +1819,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1831,22 +1831,22 @@
         <v>35</v>
       </c>
       <c r="D36" t="n">
-        <v>1.564641508472481</v>
+        <v>1.261780978028505</v>
       </c>
       <c r="E36" t="n">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="F36" t="n">
-        <v>0.08666666666666667</v>
+        <v>0.04222222222222222</v>
       </c>
       <c r="G36" t="n">
-        <v>0.2813459712801226</v>
+        <v>0.2010957636869546</v>
       </c>
       <c r="H36" t="n">
-        <v>0.8711111111111111</v>
+        <v>0.9155555555555556</v>
       </c>
       <c r="I36" t="n">
-        <v>0.8844444444444445</v>
+        <v>0.9466666666666667</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -1858,7 +1858,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1870,22 +1870,22 @@
         <v>36</v>
       </c>
       <c r="D37" t="n">
-        <v>1.543731420625169</v>
+        <v>1.261780978028505</v>
       </c>
       <c r="E37" t="n">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="F37" t="n">
-        <v>0.08666666666666667</v>
+        <v>0.03555555555555556</v>
       </c>
       <c r="G37" t="n">
-        <v>0.2813459712801226</v>
+        <v>0.1851792591644414</v>
       </c>
       <c r="H37" t="n">
-        <v>0.8444444444444444</v>
+        <v>0.9288888888888889</v>
       </c>
       <c r="I37" t="n">
-        <v>0.88</v>
+        <v>0.9511111111111111</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -1897,7 +1897,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1909,22 +1909,22 @@
         <v>37</v>
       </c>
       <c r="D38" t="n">
-        <v>1.604726682814473</v>
+        <v>1.261780978028505</v>
       </c>
       <c r="E38" t="n">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="F38" t="n">
-        <v>0.09333333333333334</v>
+        <v>0.04222222222222222</v>
       </c>
       <c r="G38" t="n">
-        <v>0.290898989723619</v>
+        <v>0.2010957636869546</v>
       </c>
       <c r="H38" t="n">
-        <v>0.8311111111111111</v>
+        <v>0.9155555555555556</v>
       </c>
       <c r="I38" t="n">
-        <v>0.8755555555555555</v>
+        <v>0.9511111111111111</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -1936,7 +1936,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1948,22 +1948,22 @@
         <v>38</v>
       </c>
       <c r="D39" t="n">
-        <v>1.623963756721791</v>
+        <v>1.292481250360576</v>
       </c>
       <c r="E39" t="n">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="F39" t="n">
-        <v>0.1155555555555556</v>
+        <v>0.04666666666666667</v>
       </c>
       <c r="G39" t="n">
-        <v>0.3196912090374123</v>
+        <v>0.210923893594085</v>
       </c>
       <c r="H39" t="n">
-        <v>0.8222222222222222</v>
+        <v>0.9066666666666666</v>
       </c>
       <c r="I39" t="n">
-        <v>0.88</v>
+        <v>0.9422222222222222</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -1975,7 +1975,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1987,22 +1987,22 @@
         <v>39</v>
       </c>
       <c r="D40" t="n">
-        <v>1.623963756721791</v>
+        <v>1.32192809488736</v>
       </c>
       <c r="E40" t="n">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="F40" t="n">
-        <v>0.09555555555555556</v>
+        <v>0.04222222222222222</v>
       </c>
       <c r="G40" t="n">
-        <v>0.2939807669865916</v>
+        <v>0.2010957636869546</v>
       </c>
       <c r="H40" t="n">
-        <v>0.8711111111111111</v>
+        <v>0.9155555555555556</v>
       </c>
       <c r="I40" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.9511111111111111</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -2014,7 +2014,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2026,22 +2026,22 @@
         <v>40</v>
       </c>
       <c r="D41" t="n">
-        <v>1.623963756721791</v>
+        <v>1.32192809488736</v>
       </c>
       <c r="E41" t="n">
-        <v>118</v>
+        <v>42</v>
       </c>
       <c r="F41" t="n">
-        <v>0.1311111111111111</v>
+        <v>0.04666666666666667</v>
       </c>
       <c r="G41" t="n">
-        <v>0.3375218328557739</v>
+        <v>0.210923893594085</v>
       </c>
       <c r="H41" t="n">
-        <v>0.8533333333333334</v>
+        <v>0.9066666666666666</v>
       </c>
       <c r="I41" t="n">
-        <v>0.8711111111111111</v>
+        <v>0.9511111111111111</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2065,22 +2065,22 @@
         <v>41</v>
       </c>
       <c r="D42" t="n">
-        <v>1.660964047443679</v>
+        <v>1.32192809488736</v>
       </c>
       <c r="E42" t="n">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="F42" t="n">
-        <v>0.09555555555555556</v>
+        <v>0.04888888888888889</v>
       </c>
       <c r="G42" t="n">
-        <v>0.2939807669865916</v>
+        <v>0.2156357239237014</v>
       </c>
       <c r="H42" t="n">
-        <v>0.8355555555555556</v>
+        <v>0.9022222222222223</v>
       </c>
       <c r="I42" t="n">
-        <v>0.8444444444444444</v>
+        <v>0.9422222222222222</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -2092,7 +2092,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2104,22 +2104,22 @@
         <v>42</v>
       </c>
       <c r="D43" t="n">
-        <v>1.564641508472481</v>
+        <v>1.261780978028505</v>
       </c>
       <c r="E43" t="n">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="F43" t="n">
-        <v>0.1044444444444445</v>
+        <v>0.04222222222222222</v>
       </c>
       <c r="G43" t="n">
-        <v>0.305836234722336</v>
+        <v>0.2010957636869547</v>
       </c>
       <c r="H43" t="n">
-        <v>0.8533333333333334</v>
+        <v>0.9244444444444444</v>
       </c>
       <c r="I43" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.9377777777777778</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -2131,7 +2131,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2143,22 +2143,22 @@
         <v>43</v>
       </c>
       <c r="D44" t="n">
-        <v>1.584962500721154</v>
+        <v>1.32192809488736</v>
       </c>
       <c r="E44" t="n">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="F44" t="n">
-        <v>0.08444444444444445</v>
+        <v>0.05333333333333334</v>
       </c>
       <c r="G44" t="n">
-        <v>0.2780531967931921</v>
+        <v>0.2246973272847029</v>
       </c>
       <c r="H44" t="n">
-        <v>0.8755555555555555</v>
+        <v>0.9111111111111111</v>
       </c>
       <c r="I44" t="n">
-        <v>0.88</v>
+        <v>0.9377777777777778</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -2170,7 +2170,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2182,22 +2182,22 @@
         <v>44</v>
       </c>
       <c r="D45" t="n">
-        <v>1.604726682814473</v>
+        <v>1.32192809488736</v>
       </c>
       <c r="E45" t="n">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="F45" t="n">
-        <v>0.09555555555555556</v>
+        <v>0.04444444444444445</v>
       </c>
       <c r="G45" t="n">
-        <v>0.2939807669865916</v>
+        <v>0.2060804110110156</v>
       </c>
       <c r="H45" t="n">
-        <v>0.8711111111111111</v>
+        <v>0.92</v>
       </c>
       <c r="I45" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.9288888888888889</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -2209,7 +2209,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2221,22 +2221,22 @@
         <v>45</v>
       </c>
       <c r="D46" t="n">
-        <v>1.604726682814473</v>
+        <v>1.32192809488736</v>
       </c>
       <c r="E46" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F46" t="n">
-        <v>0.08888888888888889</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="G46" t="n">
-        <v>0.2845832994414599</v>
+        <v>0.2290614236454256</v>
       </c>
       <c r="H46" t="n">
-        <v>0.84</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="I46" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.9377777777777778</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -2248,7 +2248,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2260,22 +2260,22 @@
         <v>46</v>
       </c>
       <c r="D47" t="n">
-        <v>1.660964047443679</v>
+        <v>1.377443751081732</v>
       </c>
       <c r="E47" t="n">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="F47" t="n">
-        <v>0.08666666666666667</v>
+        <v>0.04666666666666667</v>
       </c>
       <c r="G47" t="n">
-        <v>0.2813459712801226</v>
+        <v>0.210923893594085</v>
       </c>
       <c r="H47" t="n">
-        <v>0.8533333333333334</v>
+        <v>0.9066666666666666</v>
       </c>
       <c r="I47" t="n">
-        <v>0.8844444444444445</v>
+        <v>0.9377777777777778</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -2287,7 +2287,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2299,22 +2299,22 @@
         <v>47</v>
       </c>
       <c r="D48" t="n">
-        <v>1.642701109431122</v>
+        <v>1.403677461028799</v>
       </c>
       <c r="E48" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F48" t="n">
-        <v>0.08888888888888889</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="G48" t="n">
-        <v>0.2845832994414599</v>
+        <v>0.2290614236454256</v>
       </c>
       <c r="H48" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.9155555555555556</v>
       </c>
       <c r="I48" t="n">
-        <v>0.8844444444444445</v>
+        <v>0.9466666666666667</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -2326,7 +2326,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2338,22 +2338,22 @@
         <v>48</v>
       </c>
       <c r="D49" t="n">
-        <v>1.642701109431122</v>
+        <v>1.4036774610288</v>
       </c>
       <c r="E49" t="n">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="F49" t="n">
-        <v>0.09777777777777778</v>
+        <v>0.04222222222222222</v>
       </c>
       <c r="G49" t="n">
-        <v>0.2970139457173978</v>
+        <v>0.2010957636869546</v>
       </c>
       <c r="H49" t="n">
-        <v>0.84</v>
+        <v>0.9244444444444444</v>
       </c>
       <c r="I49" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.9377777777777778</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -2365,7 +2365,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2377,22 +2377,22 @@
         <v>49</v>
       </c>
       <c r="D50" t="n">
-        <v>1.678776002309039</v>
+        <v>1.4036774610288</v>
       </c>
       <c r="E50" t="n">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="F50" t="n">
-        <v>0.1</v>
+        <v>0.04444444444444445</v>
       </c>
       <c r="G50" t="n">
-        <v>0.3</v>
+        <v>0.2060804110110157</v>
       </c>
       <c r="H50" t="n">
-        <v>0.8444444444444444</v>
+        <v>0.9111111111111111</v>
       </c>
       <c r="I50" t="n">
-        <v>0.8533333333333334</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -2404,7 +2404,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2416,22 +2416,22 @@
         <v>50</v>
       </c>
       <c r="D51" t="n">
-        <v>1.67877600230904</v>
+        <v>1.4036774610288</v>
       </c>
       <c r="E51" t="n">
-        <v>102</v>
+        <v>40</v>
       </c>
       <c r="F51" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.04444444444444445</v>
       </c>
       <c r="G51" t="n">
-        <v>0.3169998247458331</v>
+        <v>0.2060804110110157</v>
       </c>
       <c r="H51" t="n">
-        <v>0.8088888888888889</v>
+        <v>0.92</v>
       </c>
       <c r="I51" t="n">
-        <v>0.8533333333333334</v>
+        <v>0.9288888888888889</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -2443,7 +2443,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2455,22 +2455,22 @@
         <v>51</v>
       </c>
       <c r="D52" t="n">
-        <v>1.660964047443679</v>
+        <v>1.32192809488736</v>
       </c>
       <c r="E52" t="n">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="F52" t="n">
-        <v>0.1066666666666667</v>
+        <v>0.04888888888888889</v>
       </c>
       <c r="G52" t="n">
-        <v>0.308688984074406</v>
+        <v>0.2156357239237014</v>
       </c>
       <c r="H52" t="n">
-        <v>0.8133333333333334</v>
+        <v>0.92</v>
       </c>
       <c r="I52" t="n">
-        <v>0.8577777777777778</v>
+        <v>0.9288888888888889</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -2482,7 +2482,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2494,22 +2494,22 @@
         <v>52</v>
       </c>
       <c r="D53" t="n">
-        <v>1.696158711389378</v>
+        <v>1.32192809488736</v>
       </c>
       <c r="E53" t="n">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="F53" t="n">
-        <v>0.1088888888888889</v>
+        <v>0.04444444444444445</v>
       </c>
       <c r="G53" t="n">
-        <v>0.3114997572477899</v>
+        <v>0.2060804110110157</v>
       </c>
       <c r="H53" t="n">
-        <v>0.8177777777777778</v>
+        <v>0.9377777777777778</v>
       </c>
       <c r="I53" t="n">
-        <v>0.8577777777777778</v>
+        <v>0.9288888888888889</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -2521,7 +2521,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2533,22 +2533,22 @@
         <v>53</v>
       </c>
       <c r="D54" t="n">
-        <v>1.729715809318646</v>
+        <v>1.350219859070544</v>
       </c>
       <c r="E54" t="n">
-        <v>108</v>
+        <v>48</v>
       </c>
       <c r="F54" t="n">
-        <v>0.12</v>
+        <v>0.05333333333333334</v>
       </c>
       <c r="G54" t="n">
-        <v>0.3249615361854384</v>
+        <v>0.2246973272847029</v>
       </c>
       <c r="H54" t="n">
-        <v>0.8133333333333334</v>
+        <v>0.92</v>
       </c>
       <c r="I54" t="n">
-        <v>0.84</v>
+        <v>0.9288888888888889</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -2560,7 +2560,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2572,22 +2572,22 @@
         <v>54</v>
       </c>
       <c r="D55" t="n">
-        <v>1.729715809318646</v>
+        <v>1.4036774610288</v>
       </c>
       <c r="E55" t="n">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="F55" t="n">
-        <v>0.1044444444444445</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="G55" t="n">
-        <v>0.305836234722336</v>
+        <v>0.2290614236454256</v>
       </c>
       <c r="H55" t="n">
-        <v>0.8355555555555556</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="I55" t="n">
-        <v>0.8488888888888889</v>
+        <v>0.9288888888888889</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
@@ -2599,7 +2599,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2611,22 +2611,22 @@
         <v>55</v>
       </c>
       <c r="D56" t="n">
-        <v>1.729715809318646</v>
+        <v>1.403677461028799</v>
       </c>
       <c r="E56" t="n">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="F56" t="n">
-        <v>0.1222222222222222</v>
+        <v>0.04888888888888889</v>
       </c>
       <c r="G56" t="n">
-        <v>0.3275422882885261</v>
+        <v>0.2156357239237014</v>
       </c>
       <c r="H56" t="n">
-        <v>0.8088888888888889</v>
+        <v>0.9377777777777778</v>
       </c>
       <c r="I56" t="n">
-        <v>0.88</v>
+        <v>0.9377777777777778</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -2638,7 +2638,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2650,22 +2650,22 @@
         <v>56</v>
       </c>
       <c r="D57" t="n">
-        <v>1.729715809318646</v>
+        <v>1.428990497563784</v>
       </c>
       <c r="E57" t="n">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="F57" t="n">
-        <v>0.09555555555555556</v>
+        <v>0.04444444444444445</v>
       </c>
       <c r="G57" t="n">
-        <v>0.2939807669865916</v>
+        <v>0.2060804110110157</v>
       </c>
       <c r="H57" t="n">
-        <v>0.8444444444444444</v>
+        <v>0.9377777777777778</v>
       </c>
       <c r="I57" t="n">
-        <v>0.8622222222222222</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
@@ -2677,7 +2677,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2689,22 +2689,22 @@
         <v>57</v>
       </c>
       <c r="D58" t="n">
-        <v>1.713132377351047</v>
+        <v>1.4036774610288</v>
       </c>
       <c r="E58" t="n">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="F58" t="n">
-        <v>0.1088888888888889</v>
+        <v>0.05111111111111111</v>
       </c>
       <c r="G58" t="n">
-        <v>0.3114997572477899</v>
+        <v>0.2202243524955829</v>
       </c>
       <c r="H58" t="n">
-        <v>0.8177777777777778</v>
+        <v>0.9155555555555556</v>
       </c>
       <c r="I58" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.9511111111111111</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
@@ -2716,7 +2716,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2728,22 +2728,22 @@
         <v>58</v>
       </c>
       <c r="D59" t="n">
-        <v>1.713132377351047</v>
+        <v>1.4036774610288</v>
       </c>
       <c r="E59" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="F59" t="n">
-        <v>0.08888888888888889</v>
+        <v>0.04444444444444445</v>
       </c>
       <c r="G59" t="n">
-        <v>0.2845832994414599</v>
+        <v>0.2060804110110157</v>
       </c>
       <c r="H59" t="n">
-        <v>0.8488888888888889</v>
+        <v>0.9111111111111111</v>
       </c>
       <c r="I59" t="n">
-        <v>0.88</v>
+        <v>0.9377777777777778</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
@@ -2755,7 +2755,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2767,22 +2767,22 @@
         <v>59</v>
       </c>
       <c r="D60" t="n">
-        <v>1.67877600230904</v>
+        <v>1.377443751081733</v>
       </c>
       <c r="E60" t="n">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="F60" t="n">
-        <v>0.08222222222222222</v>
+        <v>0.04888888888888889</v>
       </c>
       <c r="G60" t="n">
-        <v>0.2747029821371834</v>
+        <v>0.2156357239237014</v>
       </c>
       <c r="H60" t="n">
-        <v>0.88</v>
+        <v>0.9288888888888889</v>
       </c>
       <c r="I60" t="n">
-        <v>0.8844444444444445</v>
+        <v>0.9288888888888889</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -2794,7 +2794,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2806,22 +2806,22 @@
         <v>60</v>
       </c>
       <c r="D61" t="n">
-        <v>1.67877600230904</v>
+        <v>1.428990497563784</v>
       </c>
       <c r="E61" t="n">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="F61" t="n">
-        <v>0.08</v>
+        <v>0.04888888888888889</v>
       </c>
       <c r="G61" t="n">
-        <v>0.2712931993250107</v>
+        <v>0.2156357239237014</v>
       </c>
       <c r="H61" t="n">
-        <v>0.8844444444444445</v>
+        <v>0.92</v>
       </c>
       <c r="I61" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -2833,7 +2833,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2845,22 +2845,22 @@
         <v>61</v>
       </c>
       <c r="D62" t="n">
-        <v>1.67877600230904</v>
+        <v>1.403677461028799</v>
       </c>
       <c r="E62" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="F62" t="n">
-        <v>0.09333333333333334</v>
+        <v>0.05333333333333334</v>
       </c>
       <c r="G62" t="n">
-        <v>0.290898989723619</v>
+        <v>0.2246973272847029</v>
       </c>
       <c r="H62" t="n">
-        <v>0.8577777777777778</v>
+        <v>0.92</v>
       </c>
       <c r="I62" t="n">
-        <v>0.8844444444444445</v>
+        <v>0.9377777777777778</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -2872,7 +2872,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2884,22 +2884,22 @@
         <v>62</v>
       </c>
       <c r="D63" t="n">
-        <v>1.696158711389378</v>
+        <v>1.403677461028799</v>
       </c>
       <c r="E63" t="n">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="F63" t="n">
-        <v>0.08</v>
+        <v>0.05111111111111111</v>
       </c>
       <c r="G63" t="n">
-        <v>0.2712931993250107</v>
+        <v>0.2202243524955829</v>
       </c>
       <c r="H63" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.9066666666666666</v>
       </c>
       <c r="I63" t="n">
-        <v>0.8844444444444445</v>
+        <v>0.9377777777777778</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -2911,7 +2911,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2923,22 +2923,22 @@
         <v>63</v>
       </c>
       <c r="D64" t="n">
-        <v>1.696158711389378</v>
+        <v>1.428990497563784</v>
       </c>
       <c r="E64" t="n">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="F64" t="n">
-        <v>0.08888888888888889</v>
+        <v>0.06</v>
       </c>
       <c r="G64" t="n">
-        <v>0.2845832994414599</v>
+        <v>0.2374868417407583</v>
       </c>
       <c r="H64" t="n">
-        <v>0.8488888888888889</v>
+        <v>0.8977777777777778</v>
       </c>
       <c r="I64" t="n">
-        <v>0.8844444444444445</v>
+        <v>0.9288888888888889</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -2950,7 +2950,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2962,22 +2962,22 @@
         <v>64</v>
       </c>
       <c r="D65" t="n">
-        <v>1.713132377351047</v>
+        <v>1.428990497563784</v>
       </c>
       <c r="E65" t="n">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="F65" t="n">
-        <v>0.08222222222222222</v>
+        <v>0.04888888888888889</v>
       </c>
       <c r="G65" t="n">
-        <v>0.2747029821371834</v>
+        <v>0.2156357239237014</v>
       </c>
       <c r="H65" t="n">
-        <v>0.8444444444444444</v>
+        <v>0.9111111111111111</v>
       </c>
       <c r="I65" t="n">
-        <v>0.8844444444444445</v>
+        <v>0.9066666666666666</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
@@ -2989,7 +2989,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -3001,22 +3001,22 @@
         <v>65</v>
       </c>
       <c r="D66" t="n">
-        <v>1.642701109431122</v>
+        <v>1.4036774610288</v>
       </c>
       <c r="E66" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F66" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.07777777777777778</v>
       </c>
       <c r="G66" t="n">
-        <v>0.2642856666189957</v>
+        <v>0.2678215731820878</v>
       </c>
       <c r="H66" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.8711111111111111</v>
       </c>
       <c r="I66" t="n">
-        <v>0.8933333333333333</v>
+        <v>0.92</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
@@ -3028,7 +3028,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -3040,22 +3040,22 @@
         <v>66</v>
       </c>
       <c r="D67" t="n">
-        <v>1.604726682814473</v>
+        <v>1.377443751081733</v>
       </c>
       <c r="E67" t="n">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F67" t="n">
-        <v>0.06444444444444444</v>
+        <v>0.04666666666666667</v>
       </c>
       <c r="G67" t="n">
-        <v>0.245542986103638</v>
+        <v>0.210923893594085</v>
       </c>
       <c r="H67" t="n">
-        <v>0.88</v>
+        <v>0.9244444444444444</v>
       </c>
       <c r="I67" t="n">
-        <v>0.9022222222222223</v>
+        <v>0.9288888888888889</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
@@ -3067,7 +3067,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -3079,22 +3079,22 @@
         <v>67</v>
       </c>
       <c r="D68" t="n">
-        <v>1.584962500721153</v>
+        <v>1.428990497563784</v>
       </c>
       <c r="E68" t="n">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F68" t="n">
-        <v>0.07333333333333333</v>
+        <v>0.06444444444444444</v>
       </c>
       <c r="G68" t="n">
-        <v>0.2606828639468953</v>
+        <v>0.245542986103638</v>
       </c>
       <c r="H68" t="n">
-        <v>0.8711111111111111</v>
+        <v>0.8977777777777778</v>
       </c>
       <c r="I68" t="n">
-        <v>0.9066666666666666</v>
+        <v>0.9466666666666667</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -3106,7 +3106,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -3118,22 +3118,22 @@
         <v>68</v>
       </c>
       <c r="D69" t="n">
-        <v>1.604726682814473</v>
+        <v>1.428990497563784</v>
       </c>
       <c r="E69" t="n">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="F69" t="n">
-        <v>0.06444444444444444</v>
+        <v>0.04</v>
       </c>
       <c r="G69" t="n">
-        <v>0.245542986103638</v>
+        <v>0.1959591794226543</v>
       </c>
       <c r="H69" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.9288888888888889</v>
       </c>
       <c r="I69" t="n">
-        <v>0.9066666666666666</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -3145,7 +3145,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -3157,22 +3157,22 @@
         <v>69</v>
       </c>
       <c r="D70" t="n">
-        <v>1.62396375672179</v>
+        <v>1.377443751081732</v>
       </c>
       <c r="E70" t="n">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="F70" t="n">
-        <v>0.07111111111111111</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="G70" t="n">
-        <v>0.2570103519075726</v>
+        <v>0.1611072796479276</v>
       </c>
       <c r="H70" t="n">
-        <v>0.8844444444444445</v>
+        <v>0.9466666666666667</v>
       </c>
       <c r="I70" t="n">
-        <v>0.9066666666666666</v>
+        <v>0.9511111111111111</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
@@ -3184,7 +3184,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -3196,22 +3196,22 @@
         <v>70</v>
       </c>
       <c r="D71" t="n">
-        <v>1.604726682814473</v>
+        <v>1.32192809488736</v>
       </c>
       <c r="E71" t="n">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="F71" t="n">
-        <v>0.06888888888888889</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="G71" t="n">
-        <v>0.2532650980228883</v>
+        <v>0.1611072796479276</v>
       </c>
       <c r="H71" t="n">
-        <v>0.8711111111111111</v>
+        <v>0.9466666666666667</v>
       </c>
       <c r="I71" t="n">
-        <v>0.9111111111111111</v>
+        <v>0.96</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
@@ -3223,7 +3223,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -3235,22 +3235,22 @@
         <v>71</v>
       </c>
       <c r="D72" t="n">
-        <v>1.604726682814473</v>
+        <v>1.261780978028504</v>
       </c>
       <c r="E72" t="n">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="F72" t="n">
-        <v>0.07777777777777778</v>
+        <v>0.02222222222222222</v>
       </c>
       <c r="G72" t="n">
-        <v>0.2678215731820878</v>
+        <v>0.1474055462380178</v>
       </c>
       <c r="H72" t="n">
-        <v>0.8533333333333334</v>
+        <v>0.9555555555555556</v>
       </c>
       <c r="I72" t="n">
-        <v>0.8977777777777778</v>
+        <v>0.9644444444444444</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -3262,7 +3262,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Semente1-Regra1-B3/S23</t>
+          <t>[0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0]-CAR0-B3/S23</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -3274,22 +3274,22 @@
         <v>72</v>
       </c>
       <c r="D73" t="n">
-        <v>1.604726682814473</v>
+        <v>1.261780978028504</v>
       </c>
       <c r="E73" t="n">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="F73" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.02222222222222222</v>
       </c>
       <c r="G73" t="n">
-        <v>0.2642856666189957</v>
+        <v>0.1474055462380178</v>
       </c>
       <c r="H73" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.9555555555555556</v>
       </c>
       <c r="I73" t="n">
-        <v>0.8977777777777778</v>
+        <v>0.9644444444444444</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -3297,318 +3297,6 @@
         </is>
       </c>
       <c r="K73" t="inlineStr"/>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Semente1-Regra1-B3/S23</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>B3/S23</t>
-        </is>
-      </c>
-      <c r="C74" t="n">
-        <v>73</v>
-      </c>
-      <c r="D74" t="n">
-        <v>1.604726682814473</v>
-      </c>
-      <c r="E74" t="n">
-        <v>50</v>
-      </c>
-      <c r="F74" t="n">
-        <v>0.05555555555555555</v>
-      </c>
-      <c r="G74" t="n">
-        <v>0.2290614236454256</v>
-      </c>
-      <c r="H74" t="n">
-        <v>0.9066666666666666</v>
-      </c>
-      <c r="I74" t="n">
-        <v>0.9155555555555556</v>
-      </c>
-      <c r="J74" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K74" t="inlineStr"/>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Semente1-Regra1-B3/S23</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>B3/S23</t>
-        </is>
-      </c>
-      <c r="C75" t="n">
-        <v>74</v>
-      </c>
-      <c r="D75" t="n">
-        <v>1.543731420625168</v>
-      </c>
-      <c r="E75" t="n">
-        <v>46</v>
-      </c>
-      <c r="F75" t="n">
-        <v>0.05111111111111111</v>
-      </c>
-      <c r="G75" t="n">
-        <v>0.2202243524955829</v>
-      </c>
-      <c r="H75" t="n">
-        <v>0.9333333333333333</v>
-      </c>
-      <c r="I75" t="n">
-        <v>0.9333333333333333</v>
-      </c>
-      <c r="J75" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K75" t="inlineStr"/>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Semente1-Regra1-B3/S23</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>B3/S23</t>
-        </is>
-      </c>
-      <c r="C76" t="n">
-        <v>75</v>
-      </c>
-      <c r="D76" t="n">
-        <v>1.499999999999998</v>
-      </c>
-      <c r="E76" t="n">
-        <v>40</v>
-      </c>
-      <c r="F76" t="n">
-        <v>0.04444444444444445</v>
-      </c>
-      <c r="G76" t="n">
-        <v>0.2060804110110157</v>
-      </c>
-      <c r="H76" t="n">
-        <v>0.9377777777777778</v>
-      </c>
-      <c r="I76" t="n">
-        <v>0.9333333333333333</v>
-      </c>
-      <c r="J76" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K76" t="inlineStr"/>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>Semente1-Regra1-B3/S23</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>B3/S23</t>
-        </is>
-      </c>
-      <c r="C77" t="n">
-        <v>76</v>
-      </c>
-      <c r="D77" t="n">
-        <v>1.499999999999998</v>
-      </c>
-      <c r="E77" t="n">
-        <v>42</v>
-      </c>
-      <c r="F77" t="n">
-        <v>0.04666666666666667</v>
-      </c>
-      <c r="G77" t="n">
-        <v>0.210923893594085</v>
-      </c>
-      <c r="H77" t="n">
-        <v>0.9333333333333333</v>
-      </c>
-      <c r="I77" t="n">
-        <v>0.9422222222222222</v>
-      </c>
-      <c r="J77" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K77" t="inlineStr"/>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Semente1-Regra1-B3/S23</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>B3/S23</t>
-        </is>
-      </c>
-      <c r="C78" t="n">
-        <v>77</v>
-      </c>
-      <c r="D78" t="n">
-        <v>1.453445297804257</v>
-      </c>
-      <c r="E78" t="n">
-        <v>30</v>
-      </c>
-      <c r="F78" t="n">
-        <v>0.03333333333333333</v>
-      </c>
-      <c r="G78" t="n">
-        <v>0.1795054935711501</v>
-      </c>
-      <c r="H78" t="n">
-        <v>0.9422222222222222</v>
-      </c>
-      <c r="I78" t="n">
-        <v>0.9422222222222222</v>
-      </c>
-      <c r="J78" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K78" t="inlineStr"/>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>Semente1-Regra1-B3/S23</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>B3/S23</t>
-        </is>
-      </c>
-      <c r="C79" t="n">
-        <v>78</v>
-      </c>
-      <c r="D79" t="n">
-        <v>1.350219859070545</v>
-      </c>
-      <c r="E79" t="n">
-        <v>24</v>
-      </c>
-      <c r="F79" t="n">
-        <v>0.02666666666666667</v>
-      </c>
-      <c r="G79" t="n">
-        <v>0.1611072796479276</v>
-      </c>
-      <c r="H79" t="n">
-        <v>0.9466666666666667</v>
-      </c>
-      <c r="I79" t="n">
-        <v>0.9555555555555556</v>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K79" t="inlineStr"/>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>Semente1-Regra1-B3/S23</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>B3/S23</t>
-        </is>
-      </c>
-      <c r="C80" t="n">
-        <v>79</v>
-      </c>
-      <c r="D80" t="n">
-        <v>1.499999999999998</v>
-      </c>
-      <c r="E80" t="n">
-        <v>20</v>
-      </c>
-      <c r="F80" t="n">
-        <v>0.02222222222222222</v>
-      </c>
-      <c r="G80" t="n">
-        <v>0.1474055462380178</v>
-      </c>
-      <c r="H80" t="n">
-        <v>0.9555555555555556</v>
-      </c>
-      <c r="I80" t="n">
-        <v>0.9644444444444444</v>
-      </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K80" t="inlineStr"/>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>Semente1-Regra1-B3/S23</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>B3/S23</t>
-        </is>
-      </c>
-      <c r="C81" t="n">
-        <v>80</v>
-      </c>
-      <c r="D81" t="n">
-        <v>1.499999999999998</v>
-      </c>
-      <c r="E81" t="n">
-        <v>20</v>
-      </c>
-      <c r="F81" t="n">
-        <v>0.02222222222222222</v>
-      </c>
-      <c r="G81" t="n">
-        <v>0.1474055462380178</v>
-      </c>
-      <c r="H81" t="n">
-        <v>0.9555555555555556</v>
-      </c>
-      <c r="I81" t="n">
-        <v>0.9644444444444444</v>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K81" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>